<commit_message>
fix(import-company): make import company to standalone component
</commit_message>
<xml_diff>
--- a/public/company_data.xlsx
+++ b/public/company_data.xlsx
@@ -397,28 +397,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>code</v>
+      </c>
+      <c r="B1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
+        <v>npwp</v>
+      </c>
+      <c r="D1" t="str">
+        <v>email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>address</v>
+      </c>
+      <c r="F1" t="str">
         <v>phone</v>
       </c>
-      <c r="C1" t="str">
-        <v>email</v>
-      </c>
-      <c r="D1" t="str">
-        <v>address</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>C001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Company First</v>
+      </c>
+      <c r="C2" t="str">
+        <v>01923821093</v>
+      </c>
+      <c r="D2" t="str">
+        <v>company@test.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Jl. Soekarno Hatta</v>
+      </c>
+      <c r="F2" t="str">
+        <v>08771939021</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>